<commit_message>
Updated linssit -excel sheet
Corrected the error calculation for the last focal length.
</commit_message>
<xml_diff>
--- a/linssit_laskut.xlsx
+++ b/linssit_laskut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jyu-my.sharepoint.com/personal/lasiamni_jyu_fi/Documents/Fysiikka/Labrat/Linssit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="8_{0F784B3C-EAEC-47F5-8567-06EA4ACA9F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34DD4EE4-F074-46AD-B225-9BEE4536A548}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{0F784B3C-EAEC-47F5-8567-06EA4ACA9F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3518C03E-513C-4C6D-AE45-BC48A91BEA63}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="0" windowWidth="10815" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{E75A6C94-0CB1-4F25-8E03-F1AACEBCDE34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{E75A6C94-0CB1-4F25-8E03-F1AACEBCDE34}"/>
   </bookViews>
   <sheets>
     <sheet name="measurement-1-Jan" sheetId="1" r:id="rId1"/>
@@ -872,8 +872,8 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'236'46'0,"-161"-30"0,256 56-1638,196 46-5164,638 126 2463,7-13 3796,-927-182 723,205 41-225,915 268 2395,-1099-281-2294,244 76 7512,-369-116-6176,229 33 0,-169-37-963,676 161-2625,-346-69 531,1015 154 1224,16-69-1401,-384-17 1279,-854-134 517,1831 401 217,-1940-402 1743,252 102 1,-215-61-1525,381 94 0,2054 524-833,-2276-598-342,121 17-1433,1456 298-2100,-763-178 3000,-865-171 1190,-346-82 156,351 101 826,-347-98-336,-1 1 1,0 1 0,28 18 0,-8 2 4328,-32-25-4567,-1-1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0-1 0,7 1 0,13 3 299,134 40-579,125 25 0,-263-65 0,41 7 0,0-2 0,62-1 0,863-9 0,-949 3 0,-1 2 0,73 16 0,-69-10 0,83 7 0,170-17-1365,-269 0-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2653.28">2328 6511 24575,'178'-50'0,"249"-70"0,259-72-1638,659-176-7120,700-173 5865,689-257 2739,-1221 289-213,-41-91-316,11-48 1462,34 121 59,54 147 3665,-445 157-4503,211-29 0,-981 186 1498,112-17 4426,15 23-4973,110-40-2316,-516 88-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'236'45'0,"-161"-29"0,255 55-1638,196 46-5164,638 124 2463,6-12 3796,-925-181 723,205 41-225,913 265 2395,-1098-278-2294,245 76 7512,-369-116-6176,228 33 0,-168-36-963,675 159-2625,-346-68 531,1014 151 1224,16-67-1401,-384-17 1279,-852-133 517,1828 397 217,-1937-398 1743,251 102 1,-214-61-1525,380 92 0,2052 519-833,-2274-591-342,121 16-1433,1455 296-2100,-763-177 3000,-863-169 1190,-346-81 156,350 100 826,-346-97-336,-1 0 1,0 2 0,28 18 0,-8 2 4328,-32-25-4567,-1-1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0-1 0,7 1 0,13 3 299,134 39-579,125 25 0,-264-64 0,42 7 0,0-2 0,62-1 0,862-9 0,-948 3 0,-1 2 0,73 16 0,-69-10 0,82 6 0,171-16-1365,-269 0-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2653.28">2325 6438 24575,'178'-49'0,"248"-70"0,259-71-1638,659-174-7120,698-171 5865,688-254 2739,-1219 286-213,-41-90-316,12-48 1462,33 120 59,54 145 3665,-445 156-4503,211-30 0,-979 185 1498,111-17 4426,16 23-4973,109-40-2316,-515 87-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA023C-D5A2-44E1-89D5-3853727F8C5E}">
   <dimension ref="B2:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F44" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="L87" sqref="L87"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6640,8 +6640,8 @@
         <v>27</v>
       </c>
       <c r="T107">
-        <f>T106/COUNT(Q94:Q105)</f>
-        <v>0.58706547340736936</v>
+        <f>T106/SQRT(COUNT(Q94:Q105))</f>
+        <v>2.0336544546220789</v>
       </c>
     </row>
     <row r="112" spans="3:20" x14ac:dyDescent="0.25">
@@ -7183,21 +7183,21 @@
         <v>27</v>
       </c>
       <c r="T127">
-        <f>T126/COUNT(Q116:Q125)</f>
-        <v>0.44524912386278459</v>
+        <f>T126/SQRT(COUNT(Q116:Q125))</f>
+        <v>1.4080013576008272</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D112:K112"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="D13:K13"/>
     <mergeCell ref="M13:Q13"/>
     <mergeCell ref="D45:K45"/>
     <mergeCell ref="M45:R45"/>
     <mergeCell ref="D64:K64"/>
     <mergeCell ref="D71:K71"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D112:K112"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="D13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7206,6 +7206,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6e97b83c-3422-4b2a-8344-b05cd374bb92" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100037BF81C8A1D1547B12D0830A4E2F68D" ma:contentTypeVersion="17" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="2a287bb68b77d6240dda774b1ee6bf04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6e97b83c-3422-4b2a-8344-b05cd374bb92" xmlns:ns4="07d742ff-2160-4197-9a3e-69d7d0f0d25f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9f0c8411d5c9d4d9026269ddd12d358" ns3:_="" ns4:_="">
     <xsd:import namespace="6e97b83c-3422-4b2a-8344-b05cd374bb92"/>
@@ -7452,24 +7469,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C93349F8-9A37-4D8C-A33D-624072979DFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6e97b83c-3422-4b2a-8344-b05cd374bb92"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="07d742ff-2160-4197-9a3e-69d7d0f0d25f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6e97b83c-3422-4b2a-8344-b05cd374bb92" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C43AC3E-FC10-47F1-A56D-D368AAEA32E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A072AE93-7CB7-44D9-933C-7FEB96EA3050}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7486,29 +7511,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C43AC3E-FC10-47F1-A56D-D368AAEA32E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C93349F8-9A37-4D8C-A33D-624072979DFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6e97b83c-3422-4b2a-8344-b05cd374bb92"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="07d742ff-2160-4197-9a3e-69d7d0f0d25f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>